<commit_message>
added Optimized model slides
</commit_message>
<xml_diff>
--- a/challenger_models/models_compared.xlsx
+++ b/challenger_models/models_compared.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumita\Documents\RutgersDS\Project3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumita\Documents\RutgersDS\proj3\proj_3_NYC_apartments\challenger_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24C5CC1-0D5D-45D1-8754-DB6FD9EAB08D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B397C0EE-F395-4961-BB96-A2896278AC4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="1800" windowWidth="17505" windowHeight="9480" xr2:uid="{8EB70065-8D5D-4929-ADF3-E76A27D29C76}"/>
+    <workbookView xWindow="-28920" yWindow="-1155" windowWidth="29040" windowHeight="15990" xr2:uid="{8EB70065-8D5D-4929-ADF3-E76A27D29C76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>elasticnet</t>
   </si>
@@ -48,17 +48,23 @@
     <t>R square</t>
   </si>
   <si>
-    <t>Mean Square Error - TEST</t>
-  </si>
-  <si>
-    <t>best model</t>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Best Model</t>
+  </si>
+  <si>
+    <t>Mean Square Error - Test Data</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,14 +73,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,17 +98,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,18 +111,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,91 +453,108 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0.22611339488433399</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.786538042610191</v>
       </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0.23164832150283801</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0.78318317151566097</v>
       </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.22806394653908299</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.786538053634807</v>
       </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0.229526386067817</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>0.78516924811783595</v>
       </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>0.18586070593291301</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>0.82603919364146605</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0.49341150403947298</v>
       </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>